<commit_message>
Sensible uv pattern selected.
</commit_message>
<xml_diff>
--- a/excel/strawman.xlsx
+++ b/excel/strawman.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FTSpectrograph" sheetId="1" r:id="rId1"/>
@@ -1196,7 +1196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1378,7 +1378,7 @@
         <v>80</v>
       </c>
       <c r="D12">
-        <v>79.7</v>
+        <v>5</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -1755,7 +1755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Example instrument and data file now in Band 4 for speed. Unused files removed.
</commit_message>
<xml_diff>
--- a/excel/strawman.xlsx
+++ b/excel/strawman.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783"/>
   </bookViews>
   <sheets>
     <sheet name="FTSpectrograph" sheetId="1" r:id="rId1"/>
@@ -840,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -953,7 +953,7 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -993,7 +993,7 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1196,7 +1196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>